<commit_message>
Revert "Test: Skill System"
This reverts commit 8963cf0d7bf88e0310b108532a3093c223e2dc9c.
</commit_message>
<xml_diff>
--- a/GameData/GOSkillStatTable.xlsx
+++ b/GameData/GOSkillStatTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Epic Games\UE_5.3\GuardiansOrders\GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCD06AD-C828-4348-B349-D0CC04806809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DB9A91-7014-46BA-B5C4-D611830823C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6830" yWindow="5040" windowWidth="19340" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12340" yWindow="10250" windowWidth="34640" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GOCharacterStatTable" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Name</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -38,6 +38,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>CoolTime</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>ManaCost</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -123,14 +127,6 @@
   </si>
   <si>
     <t>DamageMultiplier</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>CoolDownTime</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>CastingTime</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1095,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1107,18 +1103,18 @@
     <col min="2" max="2" width="18.9140625" style="1" customWidth="1"/>
     <col min="3" max="4" width="15" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.1640625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="14" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.75" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.6640625" style="1"/>
+    <col min="6" max="6" width="14" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.75" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1130,18 +1126,15 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -1158,16 +1151,13 @@
       <c r="F2" s="1">
         <v>0</v>
       </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1">
         <v>1.2</v>
@@ -1185,15 +1175,12 @@
         <v>3</v>
       </c>
       <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
         <v>1.2</v>
@@ -1211,15 +1198,12 @@
         <v>7</v>
       </c>
       <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1">
         <v>1.2</v>
@@ -1237,15 +1221,12 @@
         <v>7</v>
       </c>
       <c r="G5" s="1">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1">
         <v>1.2</v>
@@ -1263,15 +1244,12 @@
         <v>30</v>
       </c>
       <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -1289,15 +1267,12 @@
         <v>0</v>
       </c>
       <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1">
         <v>1.2</v>
@@ -1315,15 +1290,12 @@
         <v>3</v>
       </c>
       <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1">
         <v>1.2</v>
@@ -1341,15 +1313,12 @@
         <v>5</v>
       </c>
       <c r="G9" s="1">
-        <v>1</v>
-      </c>
-      <c r="H9" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1">
         <v>1.2</v>
@@ -1367,15 +1336,12 @@
         <v>0</v>
       </c>
       <c r="G10" s="1">
-        <v>1</v>
-      </c>
-      <c r="H10" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1">
         <v>1.2</v>
@@ -1393,15 +1359,12 @@
         <v>15</v>
       </c>
       <c r="G11" s="1">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -1419,15 +1382,12 @@
         <v>0</v>
       </c>
       <c r="G12" s="1">
-        <v>1</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1">
         <v>1.2</v>
@@ -1445,15 +1405,12 @@
         <v>3</v>
       </c>
       <c r="G13" s="1">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1">
         <v>1.2</v>
@@ -1471,15 +1428,12 @@
         <v>5</v>
       </c>
       <c r="G14" s="1">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1">
         <v>1.2</v>
@@ -1497,15 +1451,12 @@
         <v>7</v>
       </c>
       <c r="G15" s="1">
-        <v>1</v>
-      </c>
-      <c r="H15" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16" s="1">
         <v>1.2</v>
@@ -1523,15 +1474,12 @@
         <v>30</v>
       </c>
       <c r="G16" s="1">
-        <v>1</v>
-      </c>
-      <c r="H16" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
@@ -1549,15 +1497,12 @@
         <v>0</v>
       </c>
       <c r="G17" s="1">
-        <v>1</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1">
         <v>1.2</v>
@@ -1575,15 +1520,12 @@
         <v>3</v>
       </c>
       <c r="G18" s="1">
-        <v>1</v>
-      </c>
-      <c r="H18" s="1">
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1">
         <v>1.2</v>
@@ -1601,15 +1543,12 @@
         <v>4</v>
       </c>
       <c r="G19" s="1">
-        <v>1</v>
-      </c>
-      <c r="H19" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1">
         <v>1.2</v>
@@ -1627,15 +1566,12 @@
         <v>5</v>
       </c>
       <c r="G20" s="1">
-        <v>1</v>
-      </c>
-      <c r="H20" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1">
         <v>1.2</v>
@@ -1653,9 +1589,6 @@
         <v>25</v>
       </c>
       <c r="G21" s="1">
-        <v>1</v>
-      </c>
-      <c r="H21" s="1">
         <v>80</v>
       </c>
     </row>

</xml_diff>